<commit_message>
Update code with new changes
</commit_message>
<xml_diff>
--- a/faculty_timetable.xlsx
+++ b/faculty_timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d64bf6e4947d497/Desktop/MeetingScheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_10DBAF08646580B3002BFF5146F4AC8C2AAD6426" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FA69FCA-72E4-4CBD-89DC-A30C30D18729}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_1F184DF5E391AB308A91FBD828CE1BE4F3FC329F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97F11B90-7699-4AEC-8768-404BF446AD74}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reeba Mam" sheetId="1" r:id="rId1"/>
@@ -126,16 +126,16 @@
     <t>DSA B2 (SY)</t>
   </si>
   <si>
+    <t>AAI B2 9TY)</t>
+  </si>
+  <si>
     <t>DSA (SY)</t>
   </si>
   <si>
+    <t>AAI (TY)</t>
+  </si>
+  <si>
     <t>AAI B1 (TY)</t>
-  </si>
-  <si>
-    <t>AAI B2 9TY)</t>
-  </si>
-  <si>
-    <t>AAI (TY)</t>
   </si>
   <si>
     <t>FSD B2 (TY)</t>
@@ -187,10 +187,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -221,8 +217,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,8 +261,25 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -284,19 +304,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -388,20 +395,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,150 +426,166 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="18" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="18" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="18" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="18" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="18" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="18" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,10 +599,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,16 +867,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -891,16 +917,16 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -931,16 +957,16 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -974,8 +1000,8 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -984,216 +1010,225 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="52" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A2" s="53">
         <v>0.28125</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="53">
         <v>0.32291666666666669</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+    </row>
+    <row r="3" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A3" s="53">
         <v>0.32291666666666669</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="53">
         <v>0.36458333333333331</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+    </row>
+    <row r="4" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+    </row>
+    <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="53">
         <v>0.37152777777777779</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="53">
         <v>0.41319444444444442</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+    </row>
+    <row r="6" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A6" s="53">
         <v>0.41319444444444442</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="53">
         <v>0.4548611111111111</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="15" t="s">
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="G6" s="55"/>
+      <c r="H6" s="54"/>
+    </row>
+    <row r="7" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A7" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+    </row>
+    <row r="8" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A8" s="53">
         <v>0.46180555555555558</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="53">
         <v>0.50347222222222221</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="59" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+    <row r="9" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A9" s="53">
         <v>0.50347222222222221</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="53">
         <v>0.54513888888888884</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="54"/>
+      <c r="D9" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="59" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+    <row r="10" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+    </row>
+    <row r="11" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A11" s="53">
         <v>0.55208333333333337</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="53">
         <v>0.59375</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+    </row>
+    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A12" s="53">
         <v>0.59375</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="53">
         <v>0.63541666666666663</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1201,7 +1236,7 @@
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A10:H10"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1212,11 +1247,14 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="6" width="13.7265625" customWidth="1"/>
+    <col min="8" max="8" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1269,7 +1307,7 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="9"/>
@@ -1278,16 +1316,16 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
@@ -1296,13 +1334,13 @@
       <c r="B5" s="12">
         <v>0.41319444444444442</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="13"/>
@@ -1332,16 +1370,16 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -1377,21 +1415,21 @@
         <v>25</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -1403,7 +1441,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="13"/>
@@ -1427,8 +1465,8 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1497,7 +1535,7 @@
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>28</v>
       </c>
       <c r="F3" s="9"/>
@@ -1505,16 +1543,16 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
@@ -1537,30 +1575,30 @@
       <c r="B6" s="8">
         <v>0.4548611111111111</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
@@ -1569,16 +1607,16 @@
       <c r="B8" s="12">
         <v>0.50347222222222221</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="19" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="18" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="21"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -1588,27 +1626,27 @@
         <v>0.54513888888888884</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="18" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="23"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -1617,7 +1655,7 @@
       <c r="B11" s="12">
         <v>0.59375</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -1631,7 +1669,7 @@
       <c r="B12" s="2">
         <v>0.63541666666666663</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1640,8 +1678,8 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1655,7 +1693,7 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1716,16 +1754,16 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
@@ -1735,18 +1773,18 @@
         <v>0.41319444444444442</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>35</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1757,31 +1795,31 @@
         <v>0.4548611111111111</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="48" t="s">
-        <v>36</v>
+      <c r="H6" s="41" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="49"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
@@ -1791,15 +1829,15 @@
         <v>0.50347222222222221</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="51"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="42"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -1808,28 +1846,28 @@
       <c r="B9" s="8">
         <v>0.54513888888888884</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -1838,11 +1876,11 @@
       <c r="B11" s="12">
         <v>0.59375</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>38</v>
       </c>
       <c r="F11" s="13"/>
@@ -1856,7 +1894,7 @@
       <c r="B12" s="2">
         <v>0.63541666666666663</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
@@ -1868,19 +1906,19 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1902,84 +1940,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>0.28125</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <v>0.32291666666666669</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="29">
         <v>0.32291666666666669</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="30">
         <v>0.36458333333333331</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="17" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="33">
+      <c r="A5" s="32">
         <v>0.37152777777777779</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="33">
         <v>0.41319444444444442</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="14" t="s">
         <v>40</v>
       </c>
@@ -1989,51 +2027,51 @@
       <c r="G5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="35"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="29">
         <v>0.41319444444444442</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>0.4548611111111111</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="10"/>
-      <c r="H6" s="32"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="36">
+      <c r="A8" s="35">
         <v>0.46180555555555558</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="36">
         <v>0.50347222222222221</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="14" t="s">
         <v>43</v>
       </c>
@@ -2042,58 +2080,58 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="38">
+      <c r="A9" s="37">
         <v>0.50347222222222221</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="38">
         <v>0.54513888888888884</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>43</v>
       </c>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+      <c r="A11" s="35">
         <v>0.55208333333333337</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="36">
         <v>0.59375</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="40">
+      <c r="A12" s="39">
         <v>0.59375</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="39">
         <v>0.63541666666666663</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2102,15 +2140,15 @@
       <c r="D12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A7:H7"/>
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>